<commit_message>
Fixed Updated and Processed Embeddings T-Test
</commit_message>
<xml_diff>
--- a/p_values_all-MiniLM-L12-v2_vs_all-MiniLM-L6-v2.xlsx
+++ b/p_values_all-MiniLM-L12-v2_vs_all-MiniLM-L6-v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="accuracy" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sensitivity" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="specificity" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="time" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="accuracy" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="sensitivity" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="specificity" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="time" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -449,7 +449,9 @@
           <t>No Finding</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="n">
+        <v>0.9367569209110885</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -457,7 +459,9 @@
           <t>Enlarged Cardiom.</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="n">
+        <v>3.201667760642614e-10</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -465,7 +469,9 @@
           <t>Cardiomegaly</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="n">
+        <v>9.581490542972419e-08</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -473,7 +479,9 @@
           <t>Lung Lesion</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="n">
+        <v>0.00399977760565483</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -481,7 +489,9 @@
           <t>Lung Opacity</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="n">
+        <v>0.4545840847298611</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -513,7 +523,9 @@
           <t>Atelectasis</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="n">
+        <v>0.3415990856234326</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -529,7 +541,9 @@
           <t>Pleural Effusion</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" t="n">
+        <v>0.3978889192397709</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -553,7 +567,9 @@
           <t>Support Devices</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="n">
+        <v>0.3107494374775444</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -587,7 +603,9 @@
           <t>No Finding</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="n">
+        <v>0.2315026934221536</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -595,7 +613,9 @@
           <t>Enlarged Cardiom.</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="n">
+        <v>2.09868506100729e-11</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -603,7 +623,9 @@
           <t>Cardiomegaly</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="n">
+        <v>3.716408000002603e-09</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -611,7 +633,9 @@
           <t>Lung Lesion</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="n">
+        <v>3.86073535379554e-06</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -619,7 +643,9 @@
           <t>Lung Opacity</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="n">
+        <v>0.07732544779228454</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -651,7 +677,9 @@
           <t>Atelectasis</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="n">
+        <v>0.0004986954125883854</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -667,7 +695,9 @@
           <t>Pleural Effusion</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" t="n">
+        <v>0.5340768696378337</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -691,7 +721,9 @@
           <t>Support Devices</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="n">
+        <v>0.9818449888605499</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -725,7 +757,9 @@
           <t>No Finding</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="n">
+        <v>0.376069952301525</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -733,7 +767,9 @@
           <t>Enlarged Cardiom.</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="n">
+        <v>0.02215798961689382</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -741,7 +777,9 @@
           <t>Cardiomegaly</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="n">
+        <v>0.02468624933218203</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -749,7 +787,9 @@
           <t>Lung Lesion</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="n">
+        <v>0.1291322430291489</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -757,7 +797,9 @@
           <t>Lung Opacity</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="n">
+        <v>0.003246495043908954</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -789,7 +831,9 @@
           <t>Atelectasis</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="n">
+        <v>6.098849253641642e-05</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -805,7 +849,9 @@
           <t>Pleural Effusion</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" t="n">
+        <v>0.1625510095051058</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -829,7 +875,9 @@
           <t>Support Devices</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="n">
+        <v>0.007682017017812855</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -864,7 +912,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.271955650010275e-29</v>
+        <v>2.009597066272628e-33</v>
       </c>
     </row>
     <row r="3">
@@ -874,7 +922,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4.271955650010275e-29</v>
+        <v>2.009597066272628e-33</v>
       </c>
     </row>
     <row r="4">
@@ -884,7 +932,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4.271955650010275e-29</v>
+        <v>2.009597066272628e-33</v>
       </c>
     </row>
     <row r="5">
@@ -894,7 +942,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4.271955650010275e-29</v>
+        <v>2.009597066272628e-33</v>
       </c>
     </row>
     <row r="6">
@@ -904,7 +952,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.271955650010275e-29</v>
+        <v>2.009597066272628e-33</v>
       </c>
     </row>
     <row r="7">
@@ -914,7 +962,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4.271955650010275e-29</v>
+        <v>2.009597066272628e-33</v>
       </c>
     </row>
     <row r="8">
@@ -924,7 +972,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4.271955650010275e-29</v>
+        <v>2.009597066272628e-33</v>
       </c>
     </row>
     <row r="9">
@@ -934,7 +982,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>4.271955650010275e-29</v>
+        <v>2.009597066272628e-33</v>
       </c>
     </row>
     <row r="10">
@@ -944,7 +992,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4.271955650010275e-29</v>
+        <v>2.009597066272628e-33</v>
       </c>
     </row>
     <row r="11">
@@ -954,7 +1002,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4.271955650010275e-29</v>
+        <v>2.009597066272628e-33</v>
       </c>
     </row>
     <row r="12">
@@ -964,7 +1012,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4.271955650010275e-29</v>
+        <v>2.009597066272628e-33</v>
       </c>
     </row>
     <row r="13">
@@ -974,7 +1022,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4.271955650010275e-29</v>
+        <v>2.009597066272628e-33</v>
       </c>
     </row>
     <row r="14">
@@ -984,7 +1032,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4.271955650010275e-29</v>
+        <v>2.009597066272628e-33</v>
       </c>
     </row>
     <row r="15">
@@ -994,7 +1042,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4.271955650010275e-29</v>
+        <v>2.009597066272628e-33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>